<commit_message>
Minor upate to exp spreadsheet
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -19,12 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
   <si>
-    <t>Algorithm</t>
+    <t>ND</t>
   </si>
   <si>
-    <t>Real-world</t>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Ch</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Worried</t>
   </si>
 </sst>
 </file>
@@ -53,7 +62,7 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -63,6 +72,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -88,11 +109,17 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
@@ -107,38 +134,50 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1:IV1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="21.998677884615386" customWidth="1"/>
-    <col min="2" max="5" style="0" width="9.142307692307693"/>
-    <col min="6" max="6" style="0" width="13.999158653846155" customWidth="1"/>
-    <col min="7" max="256" style="0" width="9.142307692307693"/>
+    <col min="2" max="7" style="0" width="9.142307692307693"/>
+    <col min="8" max="8" style="0" width="13.999158653846155" customWidth="1"/>
+    <col min="9" max="256" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Algorithm</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>D/ND</t>
+        </is>
+      </c>
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="E1" s="1">
         <v>5</v>
       </c>
-      <c r="D1" s="1">
+      <c r="F1" s="1">
         <v>10</v>
       </c>
-      <c r="E1" s="1">
+      <c r="G1" s="1">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Real-world</t>
+        </is>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -395,18 +434,30 @@
         </is>
       </c>
     </row>
-    <row r="3" spans="1:256">
+    <row r="3" spans="1:256" ht="13.5">
       <c r="A3" t="inlineStr">
         <is>
           <t>faber1994</t>
         </is>
       </c>
-    </row>
-    <row r="4" spans="1:256">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:256" ht="13.5">
       <c r="A4" t="inlineStr">
         <is>
           <t>hand2005</t>
         </is>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:256">
@@ -430,10 +481,15 @@
         </is>
       </c>
     </row>
-    <row r="8" spans="1:256">
+    <row r="8" spans="1:256" ht="13.5">
       <c r="A8" t="inlineStr">
         <is>
           <t>khanahmad2004</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Unfinished</t>
         </is>
       </c>
     </row>
@@ -444,17 +500,34 @@
         </is>
       </c>
     </row>
-    <row r="10" spans="1:256">
+    <row r="10" spans="1:256" ht="13.5">
       <c r="A10" t="inlineStr">
         <is>
           <t>kmeansplusplus</t>
         </is>
       </c>
-    </row>
-    <row r="11" spans="1:256">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:256" ht="13.5">
       <c r="A11" t="inlineStr">
         <is>
           <t>likas2003</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Global k-means</t>
         </is>
       </c>
     </row>
@@ -465,31 +538,65 @@
         </is>
       </c>
     </row>
-    <row r="13" spans="1:256">
+    <row r="13" spans="1:256" ht="13.5">
       <c r="A13" t="inlineStr">
         <is>
           <t>milligan1980</t>
         </is>
       </c>
-    </row>
-    <row r="14" spans="1:256">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:256" ht="13.5">
       <c r="A14" t="inlineStr">
         <is>
           <t>onoda2012ica</t>
         </is>
       </c>
-    </row>
-    <row r="15" spans="1:256">
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:256" ht="13.5">
       <c r="A15" t="inlineStr">
         <is>
           <t>onoda2012pca</t>
         </is>
       </c>
-    </row>
-    <row r="16" spans="1:256">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>D?</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:256" ht="13.5">
       <c r="A16" t="inlineStr">
         <is>
           <t>random</t>
+        </is>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor exp status updates
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -19,18 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
   <si>
     <t>ND</t>
-  </si>
-  <si>
-    <t>IP</t>
   </si>
   <si>
     <t>Ch</t>
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>D?</t>
   </si>
   <si>
     <t>Worried</t>
@@ -62,7 +65,7 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +81,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -109,7 +118,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -122,6 +131,9 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -131,21 +143,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV19"/>
+  <dimension ref="A1:IU19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="21.998677884615386" customWidth="1"/>
-    <col min="2" max="7" style="0" width="9.142307692307693"/>
-    <col min="8" max="8" style="0" width="13.999158653846155" customWidth="1"/>
-    <col min="9" max="256" style="0" width="9.142307692307693"/>
+    <col min="2" max="6" style="0" width="9.142307692307693"/>
+    <col min="7" max="7" style="0" width="13.999158653846155" customWidth="1"/>
+    <col min="8" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="13.5">
+    <row r="1" spans="1:255" ht="13.5">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Algorithm</t>
@@ -153,29 +165,29 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>D/ND</t>
+        </is>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Real-world</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Notes</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>D/ND</t>
-        </is>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Real-world</t>
         </is>
       </c>
       <c r="I1" s="1"/>
@@ -425,196 +437,296 @@
       <c r="IS1" s="1"/>
       <c r="IT1" s="1"/>
       <c r="IU1" s="1"/>
-      <c r="IV1" s="1"/>
-    </row>
-    <row r="2" spans="1:256">
+    </row>
+    <row r="2" spans="1:255">
       <c r="A2" t="inlineStr">
         <is>
           <t>erisoglu2011</t>
         </is>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="13.5">
+    <row r="3" spans="1:255" ht="13.5">
       <c r="A3" t="inlineStr">
         <is>
           <t>faber1994</t>
         </is>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:255" ht="13.5">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>hand2005</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>ND but states 100 restarts - ask Renato</t>
+        </is>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="13.5">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>hand2005</t>
-        </is>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:255" ht="13.5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hatamlou2012</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D according to my comments</t>
+        </is>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:256">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>hatamlou2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" spans="1:256">
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Slow</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:255">
       <c r="A6" t="inlineStr">
         <is>
           <t>ikmeans</t>
         </is>
       </c>
     </row>
-    <row r="7" spans="1:256">
-      <c r="A7" t="inlineStr">
+    <row r="7" spans="1:255" ht="13.5">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>khan2012</t>
         </is>
       </c>
-    </row>
-    <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" t="inlineStr">
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:255" ht="13.5">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>khanahmad2004</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="H8" s="4" t="inlineStr">
         <is>
           <t>Unfinished</t>
         </is>
       </c>
     </row>
-    <row r="9" spans="1:256">
+    <row r="9" spans="1:255" ht="13.5">
       <c r="A9" t="inlineStr">
         <is>
           <t>kkz1994</t>
         </is>
       </c>
-    </row>
-    <row r="10" spans="1:256" ht="13.5">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>D (Ch)</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:255" ht="13.5">
       <c r="A10" t="inlineStr">
         <is>
           <t>kmeansplusplus</t>
         </is>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s">
         <v>0</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:255" ht="13.5">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>likas2003</t>
+        </is>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>SLOW. Global k-means</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" spans="1:255">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>macqueen1967</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:255" ht="13.5">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>milligan1980</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Ward agglomerative clustering - ask Renato</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" spans="1:255" ht="13.5">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>onoda2012ica</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Weird</t>
+        </is>
+      </c>
+      <c r="C14"/>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:255" ht="13.5">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>onoda2012pca</t>
+        </is>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:256" ht="13.5">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>likas2003</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Global k-means</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" spans="1:256">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>macqueen1967</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" spans="1:256" ht="13.5">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>milligan1980</t>
-        </is>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:256" ht="13.5">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>onoda2012ica</t>
-        </is>
-      </c>
-      <c r="F14" t="s">
+    </row>
+    <row r="16" spans="1:255" ht="13.5">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:255" ht="13.5">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>spss2010</t>
+        </is>
+      </c>
+      <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:256" ht="13.5">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>onoda2012pca</t>
-        </is>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>D?</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" spans="1:256" ht="13.5">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" spans="1:256">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>spss2010</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" spans="1:256">
-      <c r="A18" t="inlineStr">
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Slower than some</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" spans="1:255">
+      <c r="A18" s="3" t="inlineStr">
         <is>
           <t>steinley2007</t>
         </is>
       </c>
     </row>
-    <row r="19" spans="1:256">
+    <row r="19" spans="1:255">
       <c r="A19" t="inlineStr">
         <is>
           <t>yuan2004</t>

</xml_diff>

<commit_message>
Update exp spreadsheet a little
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -19,24 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+  <si>
+    <t>bradleyfayyad1998</t>
+  </si>
   <si>
     <t>ND</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
   <si>
     <t>Ch</t>
   </si>
   <si>
-    <t>*</t>
+    <t>D</t>
   </si>
   <si>
     <t>D?</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Worried</t>
   </si>
   <si>
-    <t>Slower than some</t>
+    <t>yuan2004</t>
   </si>
 </sst>
 </file>
@@ -65,7 +74,7 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,8 +88,20 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -118,7 +139,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -134,6 +155,12 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -146,7 +173,7 @@
   <dimension ref="A1:IU19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -154,7 +181,8 @@
     <col min="1" max="1" style="0" width="21.998677884615386" customWidth="1"/>
     <col min="2" max="6" style="0" width="9.142307692307693"/>
     <col min="7" max="7" style="0" width="13.999158653846155" customWidth="1"/>
-    <col min="8" max="16384" style="0" width="9.142307692307693"/>
+    <col min="8" max="8" style="0" width="16.28473557692308" customWidth="1"/>
+    <col min="9" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="13.5">
@@ -438,305 +466,576 @@
       <c r="IT1" s="1"/>
       <c r="IU1" s="1"/>
     </row>
-    <row r="2" spans="1:255">
-      <c r="A2" t="inlineStr">
+    <row r="2" spans="1:255" ht="13.5">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BO2" s="2"/>
+      <c r="BP2" s="2"/>
+      <c r="BQ2" s="2"/>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="2"/>
+      <c r="BT2" s="2"/>
+      <c r="BU2" s="2"/>
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2"/>
+      <c r="BX2" s="2"/>
+      <c r="BY2" s="2"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+      <c r="CB2" s="2"/>
+      <c r="CC2" s="2"/>
+      <c r="CD2" s="2"/>
+      <c r="CE2" s="2"/>
+      <c r="CF2" s="2"/>
+      <c r="CG2" s="2"/>
+      <c r="CH2" s="2"/>
+      <c r="CI2" s="2"/>
+      <c r="CJ2" s="2"/>
+      <c r="CK2" s="2"/>
+      <c r="CL2" s="2"/>
+      <c r="CM2" s="2"/>
+      <c r="CN2" s="2"/>
+      <c r="CO2" s="2"/>
+      <c r="CP2" s="2"/>
+      <c r="CQ2" s="2"/>
+      <c r="CR2" s="2"/>
+      <c r="CS2" s="2"/>
+      <c r="CT2" s="2"/>
+      <c r="CU2" s="2"/>
+      <c r="CV2" s="2"/>
+      <c r="CW2" s="2"/>
+      <c r="CX2" s="2"/>
+      <c r="CY2" s="2"/>
+      <c r="CZ2" s="2"/>
+      <c r="DA2" s="2"/>
+      <c r="DB2" s="2"/>
+      <c r="DC2" s="2"/>
+      <c r="DD2" s="2"/>
+      <c r="DE2" s="2"/>
+      <c r="DF2" s="2"/>
+      <c r="DG2" s="2"/>
+      <c r="DH2" s="2"/>
+      <c r="DI2" s="2"/>
+      <c r="DJ2" s="2"/>
+      <c r="DK2" s="2"/>
+      <c r="DL2" s="2"/>
+      <c r="DM2" s="2"/>
+      <c r="DN2" s="2"/>
+      <c r="DO2" s="2"/>
+      <c r="DP2" s="2"/>
+      <c r="DQ2" s="2"/>
+      <c r="DR2" s="2"/>
+      <c r="DS2" s="2"/>
+      <c r="DT2" s="2"/>
+      <c r="DU2" s="2"/>
+      <c r="DV2" s="2"/>
+      <c r="DW2" s="2"/>
+      <c r="DX2" s="2"/>
+      <c r="DY2" s="2"/>
+      <c r="DZ2" s="2"/>
+      <c r="EA2" s="2"/>
+      <c r="EB2" s="2"/>
+      <c r="EC2" s="2"/>
+      <c r="ED2" s="2"/>
+      <c r="EE2" s="2"/>
+      <c r="EF2" s="2"/>
+      <c r="EG2" s="2"/>
+      <c r="EH2" s="2"/>
+      <c r="EI2" s="2"/>
+      <c r="EJ2" s="2"/>
+      <c r="EK2" s="2"/>
+      <c r="EL2" s="2"/>
+      <c r="EM2" s="2"/>
+      <c r="EN2" s="2"/>
+      <c r="EO2" s="2"/>
+      <c r="EP2" s="2"/>
+      <c r="EQ2" s="2"/>
+      <c r="ER2" s="2"/>
+      <c r="ES2" s="2"/>
+      <c r="ET2" s="2"/>
+      <c r="EU2" s="2"/>
+      <c r="EV2" s="2"/>
+      <c r="EW2" s="2"/>
+      <c r="EX2" s="2"/>
+      <c r="EY2" s="2"/>
+      <c r="EZ2" s="2"/>
+      <c r="FA2" s="2"/>
+      <c r="FB2" s="2"/>
+      <c r="FC2" s="2"/>
+      <c r="FD2" s="2"/>
+      <c r="FE2" s="2"/>
+      <c r="FF2" s="2"/>
+      <c r="FG2" s="2"/>
+      <c r="FH2" s="2"/>
+      <c r="FI2" s="2"/>
+      <c r="FJ2" s="2"/>
+      <c r="FK2" s="2"/>
+      <c r="FL2" s="2"/>
+      <c r="FM2" s="2"/>
+      <c r="FN2" s="2"/>
+      <c r="FO2" s="2"/>
+      <c r="FP2" s="2"/>
+      <c r="FQ2" s="2"/>
+      <c r="FR2" s="2"/>
+      <c r="FS2" s="2"/>
+      <c r="FT2" s="2"/>
+      <c r="FU2" s="2"/>
+      <c r="FV2" s="2"/>
+      <c r="FW2" s="2"/>
+      <c r="FX2" s="2"/>
+      <c r="FY2" s="2"/>
+      <c r="FZ2" s="2"/>
+      <c r="GA2" s="2"/>
+      <c r="GB2" s="2"/>
+      <c r="GC2" s="2"/>
+      <c r="GD2" s="2"/>
+      <c r="GE2" s="2"/>
+      <c r="GF2" s="2"/>
+      <c r="GG2" s="2"/>
+      <c r="GH2" s="2"/>
+      <c r="GI2" s="2"/>
+      <c r="GJ2" s="2"/>
+      <c r="GK2" s="2"/>
+      <c r="GL2" s="2"/>
+      <c r="GM2" s="2"/>
+      <c r="GN2" s="2"/>
+      <c r="GO2" s="2"/>
+      <c r="GP2" s="2"/>
+      <c r="GQ2" s="2"/>
+      <c r="GR2" s="2"/>
+      <c r="GS2" s="2"/>
+      <c r="GT2" s="2"/>
+      <c r="GU2" s="2"/>
+      <c r="GV2" s="2"/>
+      <c r="GW2" s="2"/>
+      <c r="GX2" s="2"/>
+      <c r="GY2" s="2"/>
+      <c r="GZ2" s="2"/>
+      <c r="HA2" s="2"/>
+      <c r="HB2" s="2"/>
+      <c r="HC2" s="2"/>
+      <c r="HD2" s="2"/>
+      <c r="HE2" s="2"/>
+      <c r="HF2" s="2"/>
+      <c r="HG2" s="2"/>
+      <c r="HH2" s="2"/>
+      <c r="HI2" s="2"/>
+      <c r="HJ2" s="2"/>
+      <c r="HK2" s="2"/>
+      <c r="HL2" s="2"/>
+      <c r="HM2" s="2"/>
+      <c r="HN2" s="2"/>
+      <c r="HO2" s="2"/>
+      <c r="HP2" s="2"/>
+      <c r="HQ2" s="2"/>
+      <c r="HR2" s="2"/>
+      <c r="HS2" s="2"/>
+      <c r="HT2" s="2"/>
+      <c r="HU2" s="2"/>
+      <c r="HV2" s="2"/>
+      <c r="HW2" s="2"/>
+      <c r="HX2" s="2"/>
+      <c r="HY2" s="2"/>
+      <c r="HZ2" s="2"/>
+      <c r="IA2" s="2"/>
+      <c r="IB2" s="2"/>
+      <c r="IC2" s="2"/>
+      <c r="ID2" s="2"/>
+      <c r="IE2" s="2"/>
+      <c r="IF2" s="2"/>
+      <c r="IG2" s="2"/>
+      <c r="IH2" s="2"/>
+      <c r="II2" s="2"/>
+      <c r="IJ2" s="2"/>
+      <c r="IK2" s="2"/>
+      <c r="IL2" s="2"/>
+      <c r="IM2" s="2"/>
+      <c r="IN2" s="2"/>
+      <c r="IO2" s="2"/>
+      <c r="IP2" s="2"/>
+      <c r="IQ2" s="2"/>
+      <c r="IR2" s="2"/>
+      <c r="IS2" s="2"/>
+      <c r="IT2" s="2"/>
+      <c r="IU2" s="2"/>
+    </row>
+    <row r="3" spans="1:255">
+      <c r="A3" t="inlineStr">
         <is>
           <t>erisoglu2011</t>
         </is>
-      </c>
-    </row>
-    <row r="3" spans="1:255" ht="13.5">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>faber1994</t>
-        </is>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:255" ht="13.5">
       <c r="A4" t="inlineStr">
         <is>
-          <t>hand2005</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>ND but states 100 restarts - ask Renato</t>
-        </is>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
+          <t>faber1994</t>
+        </is>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:255" ht="13.5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>hand2005</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>Revisit paper. States 100 restarts - we use 50 - but are they different?</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:255" ht="13.5">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>hatamlou2012</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>D according to my comments</t>
         </is>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>Slow</t>
         </is>
       </c>
     </row>
-    <row r="6" spans="1:255" ht="13.5">
-      <c r="A6" s="4" t="inlineStr">
+    <row r="7" spans="1:255" ht="13.5">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>ikmeans</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>Has own scaling. Need to remove.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" spans="1:255" ht="13.5">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>Has own scaling. Use ours instead. What about threshold of resolution?</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:255" ht="13.5">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>khan2012</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
         <is>
           <t>Column</t>
         </is>
       </c>
     </row>
-    <row r="8" spans="1:255" ht="13.5">
-      <c r="A8" s="4" t="inlineStr">
+    <row r="9" spans="1:255" ht="13.5">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>khanahmad2004</t>
         </is>
       </c>
-      <c r="H8" s="4" t="inlineStr">
+      <c r="H9" s="6" t="inlineStr">
         <is>
           <t>Unfinished</t>
         </is>
-      </c>
-    </row>
-    <row r="9" spans="1:255" ht="13.5">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>kkz1994</t>
-        </is>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:255" ht="13.5">
       <c r="A10" t="inlineStr">
         <is>
-          <t>kmeansplusplus</t>
+          <t>kkz1994</t>
         </is>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:255" ht="13.5">
       <c r="A11" t="inlineStr">
         <is>
+          <t>kmeansplusplus</t>
+        </is>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:255" ht="13.5">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>likas2003</t>
         </is>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>SLOW. Global k-means</t>
         </is>
       </c>
     </row>
-    <row r="12" spans="1:255">
-      <c r="A12" t="inlineStr">
+    <row r="13" spans="1:255">
+      <c r="A13" t="inlineStr">
         <is>
           <t>macqueen1967</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" spans="1:255" ht="13.5">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>milligan1980</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H13" s="3" t="inlineStr">
-        <is>
-          <t>Ward agglomerative clustering - ask Renato</t>
         </is>
       </c>
     </row>
     <row r="14" spans="1:255" ht="13.5">
       <c r="A14" t="inlineStr">
         <is>
-          <t>onoda2012ica</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Weird</t>
-        </is>
-      </c>
-      <c r="C14"/>
+          <t>milligan1980</t>
+        </is>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="E14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:255" ht="13.5">
       <c r="A15" t="inlineStr">
         <is>
-          <t>onoda2012pca</t>
+          <t>onoda2012ica</t>
         </is>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C15"/>
+      <c r="E15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:255" ht="13.5">
       <c r="A16" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>onoda2012pca</t>
         </is>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>*</t>
         </is>
       </c>
     </row>
     <row r="17" spans="1:255" ht="13.5">
       <c r="A17" t="inlineStr">
         <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" spans="1:255" ht="13.5">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>spss2010</t>
         </is>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Slower than some</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:255" ht="13.5">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:255">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>steinley2007</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" spans="1:255" ht="13.5">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>yuan2004</t>
-        </is>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="C19" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>

<commit_message>
Latest additions to exp status s/sheet
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -19,15 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
-  <si>
-    <t>bradleyfayyad1998</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
   <si>
     <t>ND</t>
-  </si>
-  <si>
-    <t>IP</t>
   </si>
   <si>
     <t>Ch</t>
@@ -39,13 +33,7 @@
     <t>D?</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Worried</t>
-  </si>
-  <si>
-    <t>yuan2004</t>
   </si>
 </sst>
 </file>
@@ -100,6 +88,12 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="none">
         <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FF000000"/>
@@ -108,12 +102,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -173,7 +161,7 @@
   <dimension ref="A1:IU19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -467,20 +455,30 @@
       <c r="IU1" s="1"/>
     </row>
     <row r="2" spans="1:255" ht="13.5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>bradleyfayyad1998</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>Hung - 74,999 (so -1!)</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Hung - 1357</t>
+        </is>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -735,6 +733,7 @@
           <t>erisoglu2011</t>
         </is>
       </c>
+      <c r="H3"/>
     </row>
     <row r="4" spans="1:255" ht="13.5">
       <c r="A4" t="inlineStr">
@@ -743,19 +742,19 @@
         </is>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:255" ht="13.5">
@@ -764,10 +763,10 @@
           <t>hand2005</t>
         </is>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="inlineStr">
         <is>
           <t>Revisit paper. States 100 restarts - we use 50 - but are they different?</t>
         </is>
@@ -785,10 +784,10 @@
         </is>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -797,42 +796,42 @@
       </c>
     </row>
     <row r="7" spans="1:255" ht="13.5">
-      <c r="A7" s="5" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>ikmeans</t>
         </is>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="5" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6" t="inlineStr">
         <is>
           <t>Has own scaling. Use ours instead. What about threshold of resolution?</t>
         </is>
       </c>
     </row>
     <row r="8" spans="1:255" ht="13.5">
-      <c r="A8" s="5" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>khan2012</t>
         </is>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="5" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="inlineStr">
         <is>
           <t>Column</t>
         </is>
       </c>
     </row>
     <row r="9" spans="1:255" ht="13.5">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>khanahmad2004</t>
         </is>
       </c>
-      <c r="H9" s="6" t="inlineStr">
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>Unfinished</t>
         </is>
@@ -845,19 +844,24 @@
         </is>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Revisit paper to be sure it's D</t>
+        </is>
       </c>
     </row>
     <row r="11" spans="1:255" ht="13.5">
@@ -867,19 +871,19 @@
         </is>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:255" ht="13.5">
@@ -889,19 +893,19 @@
         </is>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -923,21 +927,21 @@
         </is>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:255" ht="13.5">
       <c r="A15" t="inlineStr">
@@ -945,15 +949,17 @@
           <t>onoda2012ica</t>
         </is>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
       </c>
       <c r="C15"/>
-      <c r="E15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>7</v>
+      <c r="E15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:255" ht="13.5">
@@ -963,13 +969,13 @@
         </is>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -984,18 +990,18 @@
         </is>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="6" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1007,35 +1013,32 @@
           <t>spss2010</t>
         </is>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
+      <c r="B18" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:255" ht="13.5">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>yuan2004</t>
+        </is>
+      </c>
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Slower than some</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" spans="1:255" ht="13.5">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6" t="inlineStr">
+      <c r="C19" s="4" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>

<commit_message>
Get notes in order
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -22,15 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
   <si>
     <t>ND</t>
   </si>
   <si>
     <t>TBC</t>
-  </si>
-  <si>
-    <t>IP 0-37</t>
   </si>
   <si>
     <t>D</t>
@@ -110,6 +107,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -117,12 +120,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -196,8 +193,8 @@
   </sheetPr>
   <dimension ref="A1:IU19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0" tabSelected="1">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -515,8 +512,10 @@
           <t>Hung - 1357</t>
         </is>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>2</v>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>Hung - 576</t>
+        </is>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="5"/>
@@ -775,10 +774,10 @@
         </is>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
@@ -843,75 +842,77 @@
         </is>
       </c>
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>Hung - 1,280</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2 and 10 hung at 1200 labels; 20 hung at 1280</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:255" ht="13.5">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>ikmeans</t>
+        </is>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:255" ht="13.5">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>khan2012</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="inlineStr">
+        <is>
+          <t>D -&gt; ND</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>Hung - 1,280</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2 and 10 hung at 1200 labels; 20 hung at 1280</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" spans="1:255" ht="13.5">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>ikmeans</t>
-        </is>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>v1 Hung with no output</t>
-        </is>
-      </c>
-      <c r="H7" s="7" t="inlineStr">
-        <is>
-          <t>Threshold, removing small clusters</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" spans="1:255" ht="13.5">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>khan2012</t>
-        </is>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="7" t="inlineStr">
-        <is>
-          <t>Column. TODO: randomise. Becomes ND. </t>
+      <c r="E8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>Becomes ND by randomising which column is used. </t>
         </is>
       </c>
     </row>
@@ -934,7 +935,7 @@
         </is>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
@@ -948,14 +949,14 @@
       <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="8" t="inlineStr">
+      <c r="H10" s="7" t="inlineStr">
         <is>
           <t>Revisit this because Khan's explanation seems subtly different </t>
         </is>
       </c>
     </row>
     <row r="11" spans="1:255" ht="13.5">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>kmeansplusplus</t>
         </is>
@@ -983,7 +984,7 @@
         </is>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -1012,14 +1013,14 @@
         </is>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
           <t>Froze - I think at 1,000 features</t>
         </is>
       </c>
-      <c r="H13" s="7" t="inlineStr">
+      <c r="H13" s="8" t="inlineStr">
         <is>
           <t>Nb. Coarsening and Roughening</t>
         </is>
@@ -1032,7 +1033,7 @@
         </is>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
@@ -1054,26 +1055,26 @@
           <t>onoda2012ica</t>
         </is>
       </c>
-      <c r="B15" s="7" t="inlineStr">
+      <c r="B15" s="8" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>6</v>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="H15" s="7" t="inlineStr">
+      <c r="H15" s="8" t="inlineStr">
         <is>
           <t>Have been treating as D. Check this. </t>
         </is>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:255" ht="13.5">
       <c r="A16" t="inlineStr">
@@ -1082,15 +1083,15 @@
         </is>
       </c>
       <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="7" t="inlineStr">
+      <c r="E16" s="8" t="inlineStr">
         <is>
           <t>Partial output - guess same error</t>
         </is>
@@ -1152,19 +1153,19 @@
         </is>
       </c>
       <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>6</v>
+      <c r="D19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1233,8 +1234,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="8" t="s">
-        <v>6</v>
+      <c r="A4" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1253,7 +1254,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" t="inlineStr">
         <is>
           <t>Problematic</t>

</xml_diff>

<commit_message>
Update notes for ikmeans
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -113,13 +113,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -194,7 +194,7 @@
   <dimension ref="A1:IU19"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0" tabSelected="1">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -873,19 +873,25 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="5"/>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="H7" s="7" t="inlineStr">
+        <is>
+          <t>7/1500 for K=20 only find 19 clusters</t>
+        </is>
+      </c>
     </row>
     <row r="8" spans="1:255" ht="13.5">
       <c r="A8" s="6" t="inlineStr">
@@ -893,24 +899,24 @@
           <t>khan2012</t>
         </is>
       </c>
-      <c r="B8" s="8" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>D -&gt; ND</t>
         </is>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="8" t="inlineStr">
+      <c r="H8" s="7" t="inlineStr">
         <is>
           <t>Becomes ND by randomising which column is used. </t>
         </is>
@@ -949,14 +955,14 @@
       <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="7" t="inlineStr">
+      <c r="H10" s="8" t="inlineStr">
         <is>
           <t>Revisit this because Khan's explanation seems subtly different </t>
         </is>
       </c>
     </row>
     <row r="11" spans="1:255" ht="13.5">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <t>kmeansplusplus</t>
         </is>
@@ -1020,7 +1026,7 @@
           <t>Froze - I think at 1,000 features</t>
         </is>
       </c>
-      <c r="H13" s="8" t="inlineStr">
+      <c r="H13" s="7" t="inlineStr">
         <is>
           <t>Nb. Coarsening and Roughening</t>
         </is>
@@ -1055,12 +1061,12 @@
           <t>onoda2012ica</t>
         </is>
       </c>
-      <c r="B15" s="8" t="inlineStr">
+      <c r="B15" s="7" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1068,13 +1074,13 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="H15" s="8" t="inlineStr">
+      <c r="H15" s="7" t="inlineStr">
         <is>
           <t>Have been treating as D. Check this. </t>
         </is>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:255" ht="13.5">
       <c r="A16" t="inlineStr">
@@ -1091,7 +1097,7 @@
       <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="8" t="inlineStr">
+      <c r="E16" s="7" t="inlineStr">
         <is>
           <t>Partial output - guess same error</t>
         </is>
@@ -1158,13 +1164,13 @@
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1234,7 +1240,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -1254,7 +1260,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.5">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" t="inlineStr">
         <is>
           <t>Problematic</t>

</xml_diff>

<commit_message>
Note up to date after the overnight jobs
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
   <si>
     <t>ND</t>
   </si>
@@ -36,13 +36,7 @@
     <t>Errors</t>
   </si>
   <si>
-    <t>IP 1-33</t>
-  </si>
-  <si>
     <t>Slow</t>
-  </si>
-  <si>
-    <t>Slow </t>
   </si>
   <si>
     <t>Ch</t>
@@ -74,7 +68,7 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +112,18 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="none">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF000000"/>
@@ -132,12 +138,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -169,7 +169,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -209,13 +209,16 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="8" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="10" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
@@ -230,7 +233,7 @@
   <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -560,9 +563,9 @@
           <t>Hung - 576</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>IP 0-36 - at 10/411 last night</t>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>Hung at 10/411</t>
         </is>
       </c>
       <c r="H2" s="3"/>
@@ -869,7 +872,7 @@
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:256" ht="13.5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>hand2005</t>
         </is>
@@ -886,14 +889,14 @@
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="I5" s="6"/>
     </row>
@@ -912,30 +915,32 @@
       <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="8" t="inlineStr">
-        <is>
-          <t>IP 1-26*</t>
-        </is>
-      </c>
-      <c r="F6" s="8" t="inlineStr">
-        <is>
-          <t>IP 1-31</t>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Hung at 1217</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Hung at 1200</t>
         </is>
       </c>
       <c r="G6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
+        <is>
+          <t>Slow </t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
         <is>
           <t>2 and 10 hung at 1200 labels; 20 hung at 1280</t>
         </is>
       </c>
     </row>
     <row r="7" spans="1:256" ht="13.5">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>ikmeans</t>
         </is>
@@ -962,7 +967,7 @@
           <t>1 short, 10 don't complete</t>
         </is>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>7/1500 for K=20 only find 19 clusters</t>
@@ -970,33 +975,33 @@
       </c>
     </row>
     <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="12" t="inlineStr">
         <is>
           <t>khan2012</t>
         </is>
       </c>
-      <c r="B8" s="11" t="inlineStr">
+      <c r="B8" s="13" t="inlineStr">
         <is>
           <t>D -&gt; ND</t>
         </is>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11" t="inlineStr">
+      <c r="C8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="13" t="inlineStr">
         <is>
           <t>Becomes ND by randomising which column is used. </t>
         </is>
@@ -1039,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="12"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:256" ht="13.5">
       <c r="A11" s="4" t="inlineStr">
@@ -1082,23 +1087,21 @@
       <c r="D12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="7" t="inlineStr">
-        <is>
-          <t>IP 1-28 - at 1376/1288 last night</t>
-        </is>
+      <c r="E12" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>IP 0-38 - at 26/28 last night</t>
-        </is>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Hung at 27</t>
+        </is>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="11" t="inlineStr">
         <is>
           <t>Twice fell short at 1200  on 10 but was seemingly just v. Slow</t>
         </is>
@@ -1118,12 +1121,13 @@
           <t>Froze - I think at 1,000 features</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>IP 0-41</t>
-        </is>
-      </c>
-      <c r="I13" s="11" t="inlineStr">
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>At 699 after ~12 hours</t>
+        </is>
+      </c>
+      <c r="G13"/>
+      <c r="I13" s="13" t="inlineStr">
         <is>
           <t>Nb. Coarsening and Roughening</t>
         </is>
@@ -1162,26 +1166,26 @@
           <t>onoda2012ica</t>
         </is>
       </c>
-      <c r="B15" s="11" t="inlineStr">
+      <c r="B15" s="13" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>7</v>
+      <c r="C15" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="I15" s="11" t="inlineStr">
+      <c r="I15" s="13" t="inlineStr">
         <is>
           <t>Have been treating as D. Check this. </t>
         </is>
       </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:256" ht="13.5">
       <c r="A16" t="inlineStr">
@@ -1198,7 +1202,7 @@
       <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="11" t="inlineStr">
+      <c r="E16" s="13" t="inlineStr">
         <is>
           <t>Partial output - guess same error</t>
         </is>
@@ -1275,22 +1279,22 @@
           <t>Errors - rep'd on dev</t>
         </is>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="8" t="inlineStr">
-        <is>
-          <t>IP 1-39 - definitely errors</t>
-        </is>
-      </c>
-      <c r="H19" s="14" t="s">
+      <c r="D19" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>Hung at 25 with 2 exception files</t>
+        </is>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>4</v>
       </c>
       <c r="I19" s="5" t="inlineStr">
         <is>
@@ -1364,8 +1368,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
+      <c r="A4" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1384,7 +1388,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.5">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" t="inlineStr">
         <is>
           <t>Problematic</t>
@@ -1400,7 +1404,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Some fixes for duplicate candidates in Erisoglu
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="1" windowWidth="10240" windowHeight="4060"/>
+    <workbookView activeTab="0" windowWidth="10240" windowHeight="4060"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,13 @@
     <t>D</t>
   </si>
   <si>
-    <t>Errors</t>
-  </si>
-  <si>
     <t>Slow</t>
   </si>
   <si>
     <t>Ch</t>
+  </si>
+  <si>
+    <t>Errors</t>
   </si>
 </sst>
 </file>
@@ -107,6 +107,18 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor rgb="FF00CCFF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -118,20 +130,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF993366"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -203,15 +203,15 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="7" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="9" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -224,7 +224,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="11" borderId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="8" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="14" borderId="0" numFmtId="0" xfId="0">
@@ -239,10 +239,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV23"/>
+  <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -836,21 +836,13 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>Rep'd in dev</t>
+          <t>Had many errors; did work on it</t>
         </is>
       </c>
     </row>
@@ -878,10 +870,10 @@
       <c r="G4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:256" ht="13.5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>hand2005</t>
         </is>
@@ -904,8 +896,8 @@
       <c r="G5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>4</v>
+      <c r="H5" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="I5" s="6"/>
     </row>
@@ -937,7 +929,7 @@
       <c r="G6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="9" t="inlineStr">
+      <c r="H6" s="11" t="inlineStr">
         <is>
           <t>Slow </t>
         </is>
@@ -949,7 +941,7 @@
       </c>
     </row>
     <row r="7" spans="1:256" ht="13.5">
-      <c r="A7" s="10" t="inlineStr">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>ikmeans</t>
         </is>
@@ -966,7 +958,7 @@
       <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="11" t="inlineStr">
+      <c r="F7" s="12" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
@@ -976,7 +968,7 @@
           <t>1 short, 10 don't complete</t>
         </is>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>7/1500 for K=20 only find 19 clusters</t>
@@ -995,21 +987,21 @@
         </is>
       </c>
       <c r="C8" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="H8" s="7"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>Becomes ND by randomising which column is used. </t>
@@ -1052,8 +1044,8 @@
       <c r="G10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:256" ht="13.5">
       <c r="A11" s="4" t="inlineStr">
@@ -1079,7 +1071,7 @@
       <c r="G11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:256" ht="13.5">
       <c r="A12" t="inlineStr">
@@ -1108,9 +1100,9 @@
         </is>
       </c>
       <c r="H12" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="12" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="I12" s="8" t="inlineStr">
         <is>
           <t>Twice fell short at 1200  on 10 but was seemingly just v. Slow</t>
         </is>
@@ -1135,7 +1127,6 @@
           <t>At 699 after ~12 hours</t>
         </is>
       </c>
-      <c r="G13"/>
       <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Nb. Coarsening and Roughening</t>
@@ -1166,7 +1157,7 @@
       <c r="G14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:256" ht="13.5">
@@ -1181,10 +1172,10 @@
         </is>
       </c>
       <c r="C15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1209,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16" s="14" t="inlineStr">
         <is>
@@ -1246,7 +1237,7 @@
       <c r="G17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:256" ht="13.5">
       <c r="A18" s="4" t="inlineStr">
@@ -1272,7 +1263,7 @@
       <c r="G18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:256" ht="13.5">
       <c r="A19" t="inlineStr">
@@ -1289,13 +1280,13 @@
         </is>
       </c>
       <c r="D19" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19" s="5" t="inlineStr">
         <is>
@@ -1303,7 +1294,7 @@
         </is>
       </c>
       <c r="H19" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="5" t="inlineStr">
         <is>
@@ -1330,7 +1321,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1378,7 +1369,7 @@
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1416,7 +1407,7 @@
       <c r="A8" s="17"/>
     </row>
     <row r="9" spans="1:2" ht="13.5">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" t="inlineStr">
         <is>
           <t>Failures but kind of expected</t>

</xml_diff>

<commit_message>
Notes update having rerun Erisoglu with mixed success
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -130,14 +130,14 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF993366"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF993366"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -242,7 +242,7 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -828,7 +828,7 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="13.5">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>erisoglu2011</t>
         </is>
@@ -836,13 +836,26 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="I3" s="5" t="inlineStr">
-        <is>
-          <t>Had many errors; did work on it</t>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>Errors: mean of empty slice (20/28 ok)</t>
+        </is>
+      </c>
+      <c r="I3" s="8" t="inlineStr">
+        <is>
+          <t>Had many errors; work to fix it but made a couple of assumptions</t>
         </is>
       </c>
     </row>
@@ -941,7 +954,7 @@
       </c>
     </row>
     <row r="7" spans="1:256" ht="13.5">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="12" t="inlineStr">
         <is>
           <t>ikmeans</t>
         </is>
@@ -958,7 +971,7 @@
       <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="12" t="inlineStr">
+      <c r="F7" s="13" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
@@ -976,7 +989,7 @@
       </c>
     </row>
     <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" s="13" t="inlineStr">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>khan2012</t>
         </is>
@@ -986,22 +999,22 @@
           <t>D -&gt; ND</t>
         </is>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="14" t="inlineStr">
         <is>
           <t>Becomes ND by randomising which column is used. </t>
@@ -1045,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:256" ht="13.5">
       <c r="A11" s="4" t="inlineStr">
@@ -1171,7 +1184,7 @@
           <t>?</t>
         </is>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1279,13 +1292,13 @@
           <t>Errors - rep'd on dev</t>
         </is>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="5" t="inlineStr">
@@ -1368,7 +1381,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -1407,7 +1420,7 @@
       <c r="A8" s="17"/>
     </row>
     <row r="9" spans="1:2" ht="13.5">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="inlineStr">
         <is>
           <t>Failures but kind of expected</t>

</xml_diff>

<commit_message>
Performance improvements; add ugly debugging for Yuan
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -64,6 +64,16 @@
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <vertAlign val="baseline"/>
+      <sz val="10"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <vertAlign val="subscript"/>
       <sz val="10"/>
       <strike val="0"/>
     </font>
@@ -175,7 +185,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -222,6 +232,9 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="8" borderId="0" numFmtId="0" xfId="0">
@@ -242,7 +255,7 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1279,7 +1292,7 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:256" ht="13.5">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>yuan2004</t>
         </is>
@@ -1292,21 +1305,11 @@
           <t>Errors - rep'd on dev</t>
         </is>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="5" t="inlineStr">
-        <is>
-          <t>Hung at 25 with 2 exception files</t>
-        </is>
-      </c>
-      <c r="H19" s="16" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="5" t="inlineStr">
@@ -1417,7 +1420,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
     </row>
     <row r="9" spans="1:2" ht="13.5">
       <c r="A9" s="13"/>

</xml_diff>

<commit_message>
Update for separated ikmeans
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
   <si>
     <t>ND</t>
   </si>
@@ -36,7 +36,19 @@
     <t>Slow</t>
   </si>
   <si>
-    <t>khan2012</t>
+    <t>7 short</t>
+  </si>
+  <si>
+    <t>8 don't complete; errors about empty clusters</t>
+  </si>
+  <si>
+    <t>leaf is short</t>
+  </si>
+  <si>
+    <t>macqueen1967</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
   <si>
     <t>Ch</t>
@@ -144,13 +156,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF993366"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -169,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF993366"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -234,22 +246,22 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="8" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="14" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="8" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="8" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="15" borderId="0" numFmtId="0" xfId="0">
@@ -264,10 +276,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV19"/>
+  <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -981,7 +993,7 @@
     <row r="7" spans="1:256" ht="13.5">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>ikmeans</t>
+          <t>ikmeans_card</t>
         </is>
       </c>
       <c r="B7" t="s">
@@ -996,128 +1008,127 @@
       <c r="E7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="12" t="inlineStr">
-        <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>1 short, 10 don't complete</t>
-        </is>
+      <c r="F7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>7/1500 for K=20 only find 19 clusters</t>
-        </is>
+      <c r="I7" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>ikmeans_first</t>
+        </is>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="inlineStr">
+      <c r="G8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:256" ht="13.5">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>khan2012</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>D -&gt; ND</t>
         </is>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="14" t="inlineStr">
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6" t="inlineStr">
         <is>
           <t>Becomes ND by randomising which column is used. </t>
         </is>
       </c>
     </row>
-    <row r="9" spans="1:256" ht="13.5">
-      <c r="A9" s="5" t="inlineStr">
+    <row r="10" spans="1:256" ht="13.5">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>khanahmad2004</t>
         </is>
       </c>
-      <c r="I9" s="5" t="inlineStr">
+      <c r="I10" s="5" t="inlineStr">
         <is>
           <t>Unfinished; arbitrary param</t>
         </is>
       </c>
-    </row>
-    <row r="10" spans="1:256" ht="13.5">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>kkz1994</t>
-        </is>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:256" ht="13.5">
       <c r="A11" s="4" t="inlineStr">
         <is>
+          <t>kkz1994</t>
+        </is>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:256" ht="13.5">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
           <t>kmeansplusplus</t>
         </is>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:256" ht="13.5">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>likas2003</t>
-        </is>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
       <c r="C12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1130,199 +1141,221 @@
       <c r="F12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="5" t="inlineStr">
-        <is>
-          <t>Hung at 27</t>
-        </is>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>Twice fell short at 1200  on 10 but was seemingly just v. Slow</t>
-        </is>
-      </c>
+      <c r="G12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:256" ht="13.5">
       <c r="A13" t="inlineStr">
         <is>
-          <t>macqueen1967</t>
+          <t>likas2003</t>
         </is>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>Froze - I think at 1,000 features</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>At 699 after ~12 hours</t>
-        </is>
-      </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>Nb. Coarsening and Roughening</t>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Hung at 27</t>
+        </is>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="8" t="inlineStr">
+        <is>
+          <t>Twice fell short at 1200  on 10 but was seemingly just v. Slow</t>
         </is>
       </c>
     </row>
     <row r="14" spans="1:256" ht="13.5">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>milligan1980</t>
-        </is>
+      <c r="A14" t="s">
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="6"/>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Froze - I think at 1,000 features</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>At 699 after ~12 hours</t>
+        </is>
+      </c>
+      <c r="I14" s="14" t="inlineStr">
+        <is>
+          <t>Nb. Coarsening and Roughening</t>
+        </is>
+      </c>
     </row>
     <row r="15" spans="1:256" ht="13.5">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>onoda2012ica</t>
-        </is>
-      </c>
-      <c r="B15" s="14" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="I15" s="14" t="inlineStr">
-        <is>
-          <t>Have been treating as D. Check this. </t>
-        </is>
-      </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>milligan1980</t>
+        </is>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:256" ht="13.5">
       <c r="A16" t="inlineStr">
         <is>
+          <t>onoda2012ica</t>
+        </is>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="I16" s="14" t="inlineStr">
+        <is>
+          <t>Have been treating as D. Check this. </t>
+        </is>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:256" ht="13.5">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>onoda2012pca</t>
         </is>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="14" t="inlineStr">
+      <c r="C17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="14" t="inlineStr">
         <is>
           <t>Partial output - guess same error</t>
         </is>
       </c>
-      <c r="I16" s="5" t="inlineStr">
+      <c r="I17" s="5" t="inlineStr">
         <is>
           <t>Error: can't cope with more clusters than features?</t>
         </is>
       </c>
-    </row>
-    <row r="17" spans="1:256" ht="13.5">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:256" ht="13.5">
       <c r="A18" s="4" t="inlineStr">
         <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:256" ht="13.5">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
           <t>spss2010</t>
         </is>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:256" ht="13.5">
-      <c r="A19" s="5" t="inlineStr">
+      <c r="C19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:256" ht="13.5">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>yuan2004</t>
         </is>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="5" t="inlineStr">
+      <c r="C20" s="5" t="inlineStr">
         <is>
           <t>Errors - rep'd on dev</t>
         </is>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="5" t="inlineStr">
+      <c r="I20" s="5" t="inlineStr">
         <is>
           <t>Errors for 02 only the first time</t>
         </is>
@@ -1394,8 +1427,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="16" t="s">
-        <v>5</v>
+      <c r="A4" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1430,10 +1463,10 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
     </row>
     <row r="9" spans="1:2" ht="13.5">
-      <c r="A9" s="12"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="inlineStr">
         <is>
           <t>Failures but kind of expected</t>

</xml_diff>

<commit_message>
Notes up to date
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
   <si>
     <t>ND</t>
   </si>
@@ -53,6 +53,9 @@
   <si>
     <t>Errors</t>
   </si>
+  <si>
+    <t>1 short</t>
+  </si>
 </sst>
 </file>
 
@@ -259,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:IV21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0" tabSelected="1">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1148,7 +1151,7 @@
       <c r="F13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="8" t="inlineStr">
+      <c r="G13" s="3" t="inlineStr">
         <is>
           <t>Hung at 27</t>
         </is>
@@ -1292,33 +1295,33 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:256" ht="13.5">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="A19" s="8" t="inlineStr">
         <is>
           <t>spss2010</t>
         </is>
       </c>
       <c r="B19" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="3" t="inlineStr">
-        <is>
-          <t>Alg wrong</t>
+      <c r="I19" s="8" t="inlineStr">
+        <is>
+          <t>Suspect it can run out of data before finding enough clusters; have emailed author</t>
         </is>
       </c>
     </row>
@@ -1353,6 +1356,7 @@
         </is>
       </c>
     </row>
+    <row r="21" spans="1:256" ht="13.5"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>
@@ -1373,7 +1377,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Add latest notes files
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
   <si>
     <t>ND</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>1493/1500</t>
+  </si>
+  <si>
+    <t>19 ok; 8 no output; 1 (expected) exception</t>
+  </si>
+  <si>
+    <t>IP 1-33</t>
   </si>
   <si>
     <t>1200/1500</t>
@@ -106,14 +112,14 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF00"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -131,6 +137,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor rgb="FF00CCFF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -138,12 +150,6 @@
     <fill>
       <patternFill patternType="none">
         <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -221,10 +227,10 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="9" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="10" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0">
@@ -248,10 +254,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV20"/>
+  <dimension ref="A1:IW20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -261,14 +267,15 @@
     <col min="3" max="3" style="0" width="14.713401442307694" customWidth="1"/>
     <col min="4" max="4" style="0" width="13.999158653846155" customWidth="1"/>
     <col min="5" max="5" style="0" width="14.28485576923077" customWidth="1"/>
-    <col min="6" max="6" style="0" width="14.42770432692308" customWidth="1"/>
+    <col min="6" max="6" style="0" width="9.713701923076924" customWidth="1"/>
     <col min="7" max="7" style="0" width="13.999158653846155" customWidth="1"/>
-    <col min="8" max="8" style="0" width="7.9995192307692315" customWidth="1"/>
-    <col min="9" max="9" style="0" width="16.28473557692308" customWidth="1"/>
-    <col min="10" max="16384" style="0" width="9.142307692307693"/>
+    <col min="8" max="8" style="0" width="9.142307692307693"/>
+    <col min="9" max="9" style="0" width="7.9995192307692315" customWidth="1"/>
+    <col min="10" max="10" style="0" width="16.28473557692308" customWidth="1"/>
+    <col min="11" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="13.5">
+    <row r="1" spans="1:257" ht="13.5">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Algorithm</t>
@@ -296,17 +303,21 @@
           <t>Real-world</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>RW2</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Perf</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -553,8 +564,9 @@
       <c r="IT1" s="1"/>
       <c r="IU1" s="1"/>
       <c r="IV1" s="1"/>
-    </row>
-    <row r="2" spans="1:256" ht="13.5">
+      <c r="IW1" s="1"/>
+    </row>
+    <row r="2" spans="1:257" ht="13.5">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>bradleyfayyad1998</t>
@@ -578,13 +590,13 @@
       <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>Infinite loop...</t>
         </is>
       </c>
-      <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -831,9 +843,10 @@
       <c r="IT2" s="4"/>
       <c r="IU2" s="4"/>
       <c r="IV2" s="4"/>
-    </row>
-    <row r="3" spans="1:256" ht="13.5">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="IW2" s="4"/>
+    </row>
+    <row r="3" spans="1:257" ht="13.5">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>erisoglu2011</t>
         </is>
@@ -858,13 +871,18 @@
           <t>Errors: mean of empty slice (20/28 ok)</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>21/28 ok</t>
+        </is>
+      </c>
+      <c r="J3" s="6" t="inlineStr">
         <is>
           <t>Had many errors; work to fix it but made a couple of assumptions</t>
         </is>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="13.5">
+    <row r="4" spans="1:257" ht="13.5">
       <c r="A4" s="7" t="inlineStr">
         <is>
           <t>faber1994</t>
@@ -888,38 +906,46 @@
       <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:256" ht="13.5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="H4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:257" ht="13.5">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>hand2005</t>
         </is>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>3</v>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="inlineStr">
+        <is>
+          <t>Errors but no exception files</t>
+        </is>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:256" ht="13.5">
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:257" ht="13.5">
       <c r="A6" s="7" t="inlineStr">
         <is>
           <t>hatamlou2012</t>
@@ -943,15 +969,18 @@
       <c r="G6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="12" t="inlineStr">
         <is>
           <t>Slow (days!)</t>
         </is>
       </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:256" ht="13.5">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:257" ht="13.5">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>ikmeans_card</t>
         </is>
@@ -971,16 +1000,17 @@
       <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="12" t="inlineStr">
-        <is>
-          <t>IP 0-36</t>
-        </is>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="G7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:257" ht="13.5">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>ikmeans_first</t>
         </is>
@@ -1000,21 +1030,24 @@
       <c r="F8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="12" t="inlineStr">
+      <c r="G8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>IP 1-34</t>
         </is>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:256" ht="13.5">
+      <c r="I8" s="9"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:257" ht="13.5">
       <c r="A9" s="7" t="inlineStr">
         <is>
           <t>khan2012</t>
         </is>
       </c>
-      <c r="B9" s="10" t="inlineStr">
+      <c r="B9" s="11" t="inlineStr">
         <is>
           <t>D -&gt; ND</t>
         </is>
@@ -1034,26 +1067,27 @@
       <c r="G9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="10" t="inlineStr">
+      <c r="H9" s="10"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="11" t="inlineStr">
         <is>
           <t>Becomes ND by randomising which column is used. </t>
         </is>
       </c>
     </row>
-    <row r="10" spans="1:256" ht="13.5">
+    <row r="10" spans="1:257" ht="13.5">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>khanahmad2004</t>
         </is>
       </c>
-      <c r="I10" s="12" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>Unfinished; arbitrary param</t>
         </is>
       </c>
     </row>
-    <row r="11" spans="1:256" ht="13.5">
+    <row r="11" spans="1:257" ht="13.5">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>kkz1994</t>
@@ -1077,10 +1111,15 @@
       <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:256" ht="13.5">
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>IP 0-28</t>
+        </is>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:257" ht="13.5">
       <c r="A12" s="7" t="inlineStr">
         <is>
           <t>kmeansplusplus</t>
@@ -1104,9 +1143,10 @@
       <c r="G12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:256" ht="13.5">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:257" ht="13.5">
       <c r="A13" s="7" t="inlineStr">
         <is>
           <t>likas2003</t>
@@ -1130,16 +1170,17 @@
       <c r="G13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="12" t="inlineStr">
+      <c r="J13" s="9" t="inlineStr">
         <is>
           <t>Hung at 27 RW for a long time</t>
         </is>
       </c>
     </row>
-    <row r="14" spans="1:256" ht="13.5">
+    <row r="14" spans="1:257" ht="13.5">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>milligan1980</t>
@@ -1163,45 +1204,45 @@
       <c r="G14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:256" ht="13.5">
-      <c r="A15" t="inlineStr">
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:257" ht="13.5">
+      <c r="A15" s="13" t="inlineStr">
         <is>
           <t>onoda2012ica</t>
         </is>
       </c>
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+      <c r="B15" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="D15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="5" t="inlineStr">
+      <c r="E15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="J15" s="6" t="inlineStr">
         <is>
           <t>Have been treating as D. Check this. </t>
         </is>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:256" ht="13.5">
-      <c r="A16" t="inlineStr">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:257" ht="13.5">
+      <c r="A16" s="13" t="inlineStr">
         <is>
           <t>onoda2012pca</t>
         </is>
@@ -1213,24 +1254,25 @@
         <v>3</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="13" t="inlineStr">
+        <v>10</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="J16" s="13" t="inlineStr">
         <is>
           <t>Problems where n_components &gt; n_features</t>
         </is>
       </c>
     </row>
-    <row r="17" spans="1:256" ht="13.5">
+    <row r="17" spans="1:257" ht="13.5">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>random</t>
@@ -1254,25 +1296,26 @@
       <c r="G17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:256" ht="13.5">
-      <c r="A18" s="12" t="inlineStr">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:257" ht="13.5">
+      <c r="A18" s="13" t="inlineStr">
         <is>
           <t>spss2010</t>
         </is>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>3</v>
@@ -1280,14 +1323,15 @@
       <c r="G18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="12" t="inlineStr">
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="9" t="inlineStr">
         <is>
           <t>Can run out of data before finding enough clusters; have emailed author</t>
         </is>
       </c>
     </row>
-    <row r="19" spans="1:256" ht="13.5">
+    <row r="19" spans="1:257" ht="13.5">
       <c r="A19" s="7" t="inlineStr">
         <is>
           <t>yuan2004</t>
@@ -1311,14 +1355,15 @@
       <c r="G19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12" t="inlineStr">
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="inlineStr">
         <is>
           <t>Fixed bug :)</t>
         </is>
       </c>
     </row>
-    <row r="20" spans="1:256" ht="13.5"/>
+    <row r="20" spans="1:257" ht="13.5"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>
@@ -1339,7 +1384,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1405,7 +1450,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.5">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" t="inlineStr">
         <is>
           <t>Problematic</t>
@@ -1427,7 +1472,7 @@
       <c r="A9" s="13"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Experiments run; failures but possibly expected</t>
+          <t>Experiments run; failures against certain datasets, but these tend to be expected</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Status update after a day rerunning experiments
</commit_message>
<xml_diff>
--- a/_notes/status_exp.xlsx
+++ b/_notes/status_exp.xlsx
@@ -22,7 +22,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34" count="34">
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>D/ND</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Perf</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>bradleyfayyad1998</t>
+  </si>
   <si>
     <t>ND</t>
   </si>
@@ -30,24 +48,60 @@
     <t>Ch</t>
   </si>
   <si>
+    <t>erisoglu2011</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
     <t>TBC</t>
   </si>
   <si>
+    <t>faber1994</t>
+  </si>
+  <si>
+    <t>hand2005</t>
+  </si>
+  <si>
     <t>Slow</t>
   </si>
   <si>
     <t>hatamlou2012</t>
   </si>
   <si>
+    <t>ikmeans_card</t>
+  </si>
+  <si>
     <t>1493/1500</t>
   </si>
   <si>
     <t>19 ok; 8 no output; 1 (expected) exception</t>
   </si>
   <si>
+    <t>ikmeans_first</t>
+  </si>
+  <si>
+    <t>khan2012</t>
+  </si>
+  <si>
+    <t>D -&gt; ND</t>
+  </si>
+  <si>
+    <t>kkz1994</t>
+  </si>
+  <si>
+    <t>kmeansplusplus</t>
+  </si>
+  <si>
+    <t>likas2003</t>
+  </si>
+  <si>
+    <t>milligan1980</t>
+  </si>
+  <si>
+    <t>onoda2012ica</t>
+  </si>
+  <si>
     <t>1200/1500</t>
   </si>
   <si>
@@ -57,7 +111,19 @@
     <t>23/28</t>
   </si>
   <si>
+    <t>onoda2012pca</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>spss2010</t>
+  </si>
+  <si>
     <t>1499/1500</t>
+  </si>
+  <si>
+    <t>yuan2004</t>
   </si>
 </sst>
 </file>
@@ -266,7 +332,7 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -277,22 +343,18 @@
     <col min="4" max="4" style="0" width="13.999158653846155" customWidth="1"/>
     <col min="5" max="5" style="0" width="14.28485576923077" customWidth="1"/>
     <col min="6" max="6" style="0" width="9.713701923076924" customWidth="1"/>
-    <col min="7" max="7" style="0" width="20.713040865384617" customWidth="1"/>
+    <col min="7" max="7" style="0" width="10.427944711538462" customWidth="1"/>
     <col min="8" max="8" style="0" width="7.9995192307692315" customWidth="1"/>
     <col min="9" max="9" style="0" width="23.284314903846155" customWidth="1"/>
     <col min="10" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="13.5">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Algorithm</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>D/ND</t>
-        </is>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="1">
         <v>2</v>
@@ -306,20 +368,14 @@
       <c r="F1" s="1">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Real</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Perf</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -570,25 +626,23 @@
       <c r="IV1" s="1"/>
     </row>
     <row r="2" spans="1:256" ht="13.5">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>bradleyfayyad1998</t>
-        </is>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="4"/>
@@ -846,25 +900,23 @@
       <c r="IV2" s="4"/>
     </row>
     <row r="3" spans="1:256" ht="13.5">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>erisoglu2011</t>
-        </is>
+      <c r="A3" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G3" s="7" t="inlineStr">
         <is>
@@ -878,57 +930,53 @@
       </c>
     </row>
     <row r="4" spans="1:256" ht="13.5">
-      <c r="A4" s="6" t="inlineStr">
-        <is>
-          <t>faber1994</t>
-        </is>
+      <c r="A4" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:256" ht="13.5">
-      <c r="A5" s="10" t="inlineStr">
-        <is>
-          <t>hand2005</t>
-        </is>
+      <c r="A5" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="I5" s="11" t="inlineStr">
         <is>
@@ -938,25 +986,25 @@
     </row>
     <row r="6" spans="1:256" ht="13.5">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H6" s="12" t="inlineStr">
         <is>
@@ -966,84 +1014,76 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:256" ht="13.5">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>ikmeans_card</t>
-        </is>
+      <c r="A7" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>ikmeans_first</t>
-        </is>
+      <c r="A8" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:256" ht="13.5">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>khan2012</t>
-        </is>
-      </c>
-      <c r="B9" s="11" t="inlineStr">
-        <is>
-          <t>D -&gt; ND</t>
-        </is>
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="11" t="inlineStr">
@@ -1053,84 +1093,78 @@
       </c>
     </row>
     <row r="10" spans="1:256" ht="13.5">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>kkz1994</t>
-        </is>
+      <c r="A10" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:256" ht="13.5">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>kmeansplusplus</t>
-        </is>
+      <c r="A11" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:256" ht="13.5">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>likas2003</t>
-        </is>
+      <c r="A12" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="I12" s="13" t="inlineStr">
         <is>
@@ -1139,55 +1173,51 @@
       </c>
     </row>
     <row r="13" spans="1:256" ht="13.5">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>milligan1980</t>
-        </is>
+      <c r="A13" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:256" ht="13.5">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>onoda2012ica</t>
-        </is>
+      <c r="A14" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I14" s="16" t="inlineStr">
         <is>
@@ -1198,84 +1228,78 @@
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:256" ht="13.5">
-      <c r="A15" s="6" t="inlineStr">
-        <is>
-          <t>onoda2012pca</t>
-        </is>
+      <c r="A15" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="16" t="inlineStr">
+        <is>
+          <t>Problems where n_components &gt; n_features</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:256" ht="13.5">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:256" ht="13.5">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="16" t="inlineStr">
-        <is>
-          <t>Problems where n_components &gt; n_features</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" spans="1:256" ht="13.5">
-      <c r="A16" s="6" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:256" ht="13.5">
-      <c r="A17" s="6" t="inlineStr">
-        <is>
-          <t>spss2010</t>
-        </is>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="C17" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="13" t="inlineStr">
@@ -1285,28 +1309,26 @@
       </c>
     </row>
     <row r="18" spans="1:256" ht="13.5">
-      <c r="A18" s="6" t="inlineStr">
-        <is>
-          <t>yuan2004</t>
-        </is>
+      <c r="A18" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13" t="inlineStr">
@@ -1383,7 +1405,7 @@
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1393,7 +1415,7 @@
     </row>
     <row r="5" spans="1:2" ht="13.5">
       <c r="A5" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>

</xml_diff>